<commit_message>
Cleaned up Pedersen and included a test spreadsheet, whihc is stil not working fully.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Inflation/InflationAssets.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Inflation/InflationAssets.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2017\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Inflation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Inflation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE061071-8BC7-46D1-A5F7-8922C4EB93ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FC928F-114C-491B-AE21-64A340C698F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="12315" windowHeight="13035" tabRatio="416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="0" windowWidth="26370" windowHeight="14820" tabRatio="416" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Curves" sheetId="2" r:id="rId1"/>
     <sheet name="Priceable Inflation Assets" sheetId="4" r:id="rId2"/>
     <sheet name="Daily Forward Rates" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2407,301 +2415,301 @@
                 <c:formatCode>d/m/yyyy;@</c:formatCode>
                 <c:ptCount val="99"/>
                 <c:pt idx="0">
-                  <c:v>43215</c:v>
+                  <c:v>43640</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43216</c:v>
+                  <c:v>43641</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43217</c:v>
+                  <c:v>43642</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43218</c:v>
+                  <c:v>43643</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43219</c:v>
+                  <c:v>43644</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43220</c:v>
+                  <c:v>43645</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43221</c:v>
+                  <c:v>43646</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43222</c:v>
+                  <c:v>43647</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43223</c:v>
+                  <c:v>43648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43224</c:v>
+                  <c:v>43649</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43225</c:v>
+                  <c:v>43650</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43226</c:v>
+                  <c:v>43651</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43227</c:v>
+                  <c:v>43652</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43228</c:v>
+                  <c:v>43653</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43229</c:v>
+                  <c:v>43654</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43230</c:v>
+                  <c:v>43655</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43231</c:v>
+                  <c:v>43656</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43232</c:v>
+                  <c:v>43657</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>43233</c:v>
+                  <c:v>43658</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43234</c:v>
+                  <c:v>43659</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>43235</c:v>
+                  <c:v>43660</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>43236</c:v>
+                  <c:v>43661</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43237</c:v>
+                  <c:v>43662</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43238</c:v>
+                  <c:v>43663</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>43239</c:v>
+                  <c:v>43664</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>43240</c:v>
+                  <c:v>43665</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43241</c:v>
+                  <c:v>43666</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>43242</c:v>
+                  <c:v>43667</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>43243</c:v>
+                  <c:v>43668</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>43244</c:v>
+                  <c:v>43669</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43245</c:v>
+                  <c:v>43670</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>43246</c:v>
+                  <c:v>43671</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>43247</c:v>
+                  <c:v>43672</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>43248</c:v>
+                  <c:v>43673</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>43249</c:v>
+                  <c:v>43674</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>43250</c:v>
+                  <c:v>43675</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>43251</c:v>
+                  <c:v>43676</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>43252</c:v>
+                  <c:v>43677</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>43253</c:v>
+                  <c:v>43678</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>43254</c:v>
+                  <c:v>43679</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>43255</c:v>
+                  <c:v>43680</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>43256</c:v>
+                  <c:v>43681</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>43257</c:v>
+                  <c:v>43682</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>43258</c:v>
+                  <c:v>43683</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>43259</c:v>
+                  <c:v>43684</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>43260</c:v>
+                  <c:v>43685</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>43261</c:v>
+                  <c:v>43686</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>43262</c:v>
+                  <c:v>43687</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>43263</c:v>
+                  <c:v>43688</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>43264</c:v>
+                  <c:v>43689</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>43265</c:v>
+                  <c:v>43690</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>43266</c:v>
+                  <c:v>43691</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>43267</c:v>
+                  <c:v>43692</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>43268</c:v>
+                  <c:v>43693</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>43269</c:v>
+                  <c:v>43694</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>43270</c:v>
+                  <c:v>43695</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>43271</c:v>
+                  <c:v>43696</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>43272</c:v>
+                  <c:v>43697</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>43273</c:v>
+                  <c:v>43698</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>43274</c:v>
+                  <c:v>43699</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>43275</c:v>
+                  <c:v>43700</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>43276</c:v>
+                  <c:v>43701</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>43277</c:v>
+                  <c:v>43702</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>43278</c:v>
+                  <c:v>43703</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>43279</c:v>
+                  <c:v>43704</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>43280</c:v>
+                  <c:v>43705</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>43281</c:v>
+                  <c:v>43706</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>43282</c:v>
+                  <c:v>43707</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>43283</c:v>
+                  <c:v>43708</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>43284</c:v>
+                  <c:v>43709</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>43285</c:v>
+                  <c:v>43710</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>43286</c:v>
+                  <c:v>43711</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>43287</c:v>
+                  <c:v>43712</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>43288</c:v>
+                  <c:v>43713</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>43289</c:v>
+                  <c:v>43714</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>43290</c:v>
+                  <c:v>43715</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>43291</c:v>
+                  <c:v>43716</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>43292</c:v>
+                  <c:v>43717</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>43293</c:v>
+                  <c:v>43718</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>43294</c:v>
+                  <c:v>43719</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>43295</c:v>
+                  <c:v>43720</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>43296</c:v>
+                  <c:v>43721</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>43297</c:v>
+                  <c:v>43722</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>43298</c:v>
+                  <c:v>43723</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>43299</c:v>
+                  <c:v>43724</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>43300</c:v>
+                  <c:v>43725</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>43301</c:v>
+                  <c:v>43726</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>43302</c:v>
+                  <c:v>43727</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>43303</c:v>
+                  <c:v>43728</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>43304</c:v>
+                  <c:v>43729</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>43305</c:v>
+                  <c:v>43730</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>43306</c:v>
+                  <c:v>43731</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>43307</c:v>
+                  <c:v>43732</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>43308</c:v>
+                  <c:v>43733</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>43309</c:v>
+                  <c:v>43734</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>43310</c:v>
+                  <c:v>43735</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>43311</c:v>
+                  <c:v>43736</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>43312</c:v>
+                  <c:v>43737</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>43313</c:v>
+                  <c:v>43738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2806,208 +2814,208 @@
                   <c:v>2.9854993323920054E-2</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9850215165305727E-2</c:v>
+                  <c:v>2.9850219315280535E-2</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9845320876650816E-2</c:v>
+                  <c:v>2.9845325293673119E-2</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.984042738938153E-2</c:v>
+                  <c:v>2.9840432073289236E-2</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.983553470313316E-2</c:v>
+                  <c:v>2.9835539654047838E-2</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9830642817986752E-2</c:v>
+                  <c:v>2.9830648035665264E-2</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9825751733618122E-2</c:v>
+                  <c:v>2.982575721810099E-2</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9820861449865177E-2</c:v>
+                  <c:v>2.9820867201111878E-2</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9815971966606347E-2</c:v>
+                  <c:v>2.9815977984495312E-2</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9811083283760587E-2</c:v>
+                  <c:v>2.9811089568210769E-2</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.980619540100371E-2</c:v>
+                  <c:v>2.9806201951974587E-2</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9801308318295194E-2</c:v>
+                  <c:v>2.9801315135705719E-2</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9796422035351378E-2</c:v>
+                  <c:v>2.9796429119161028E-2</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9791536552131737E-2</c:v>
+                  <c:v>2.9791543902218942E-2</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9786651868433656E-2</c:v>
+                  <c:v>2.9786659484798417E-2</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9781767984054519E-2</c:v>
+                  <c:v>2.9781775866615789E-2</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9776884898832234E-2</c:v>
+                  <c:v>2.9776893047549491E-2</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9772002612685755E-2</c:v>
+                  <c:v>2.9772011027396905E-2</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9767121125331419E-2</c:v>
+                  <c:v>2.9767129806117509E-2</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9762240436688181E-2</c:v>
+                  <c:v>2.9762249383387118E-2</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.975736054663447E-2</c:v>
+                  <c:v>2.9757369759124686E-2</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9752481454846103E-2</c:v>
+                  <c:v>2.9752490933168119E-2</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9747603161323077E-2</c:v>
+                  <c:v>2.9747612905395848E-2</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.974272566574121E-2</c:v>
+                  <c:v>2.9742735675564735E-2</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9737848968181546E-2</c:v>
+                  <c:v>2.9737859243512688E-2</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9732973068238855E-2</c:v>
+                  <c:v>2.9732983609158659E-2</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9728097965872613E-2</c:v>
+                  <c:v>2.9728108772218986E-2</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9723223660880205E-2</c:v>
+                  <c:v>2.9723234732653148E-2</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9718350153099538E-2</c:v>
+                  <c:v>2.9718361490218004E-2</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9713477442368519E-2</c:v>
+                  <c:v>2.9713489044751462E-2</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9708605528525056E-2</c:v>
+                  <c:v>2.9708617396172476E-2</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.970373441144758E-2</c:v>
+                  <c:v>2.9703746544197385E-2</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9699116165411987E-2</c:v>
+                  <c:v>2.9698876488785664E-2</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9694254730974201E-2</c:v>
+                  <c:v>2.9694007229694175E-2</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9689394090789967E-2</c:v>
+                  <c:v>2.9689403146496152E-2</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9684534244697192E-2</c:v>
+                  <c:v>2.9684543697732768E-2</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9679675192655353E-2</c:v>
+                  <c:v>2.9679685042777182E-2</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9674816934299741E-2</c:v>
+                  <c:v>2.967482718158887E-2</c:v>
                 </c:pt>
                 <c:pt idx="68" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9669959469589835E-2</c:v>
+                  <c:v>2.96699701137626E-2</c:v>
                 </c:pt>
                 <c:pt idx="69" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9665102798282494E-2</c:v>
+                  <c:v>2.9665113839419943E-2</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9660246920337197E-2</c:v>
+                  <c:v>2.9660258358155667E-2</c:v>
                 </c:pt>
                 <c:pt idx="71" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9655391835470279E-2</c:v>
+                  <c:v>2.9655403670050817E-2</c:v>
                 </c:pt>
                 <c:pt idx="72" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9650537543560174E-2</c:v>
+                  <c:v>2.9650549774700163E-2</c:v>
                 </c:pt>
                 <c:pt idx="73" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9645684044444787E-2</c:v>
+                  <c:v>2.9645696672144228E-2</c:v>
                 </c:pt>
                 <c:pt idx="74" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9640831338043072E-2</c:v>
+                  <c:v>2.964084436209935E-2</c:v>
                 </c:pt>
                 <c:pt idx="75" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9635979424111891E-2</c:v>
+                  <c:v>2.9635992844484482E-2</c:v>
                 </c:pt>
                 <c:pt idx="76" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9631128302448628E-2</c:v>
+                  <c:v>2.9631142119015963E-2</c:v>
                 </c:pt>
                 <c:pt idx="77" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9626277972972237E-2</c:v>
+                  <c:v>2.9626292185612746E-2</c:v>
                 </c:pt>
                 <c:pt idx="78" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9621428435480102E-2</c:v>
+                  <c:v>2.9621443044112739E-2</c:v>
                 </c:pt>
                 <c:pt idx="79" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.961657968981013E-2</c:v>
+                  <c:v>2.9616594694394371E-2</c:v>
                 </c:pt>
                 <c:pt idx="80" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9611731735759705E-2</c:v>
+                  <c:v>2.9611747136214506E-2</c:v>
                 </c:pt>
                 <c:pt idx="81" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9606884573328829E-2</c:v>
+                  <c:v>2.9606900369451572E-2</c:v>
                 </c:pt>
                 <c:pt idx="82" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9602038202233838E-2</c:v>
+                  <c:v>2.9602054394024524E-2</c:v>
                 </c:pt>
                 <c:pt idx="83" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9597192622231594E-2</c:v>
+                  <c:v>2.959720920952813E-2</c:v>
                 </c:pt>
                 <c:pt idx="84" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.959234783336262E-2</c:v>
+                  <c:v>2.9592364816002914E-2</c:v>
                 </c:pt>
                 <c:pt idx="85" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9587503835262208E-2</c:v>
+                  <c:v>2.9587521213327306E-2</c:v>
                 </c:pt>
                 <c:pt idx="86" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9582660627930357E-2</c:v>
+                  <c:v>2.958267840117712E-2</c:v>
                 </c:pt>
                 <c:pt idx="87" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9577818211083406E-2</c:v>
+                  <c:v>2.9577836379471312E-2</c:v>
                 </c:pt>
                 <c:pt idx="88" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9572976584559263E-2</c:v>
+                  <c:v>2.957299514808831E-2</c:v>
                 </c:pt>
                 <c:pt idx="89" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.956813574839845E-2</c:v>
+                  <c:v>2.9568154706906546E-2</c:v>
                 </c:pt>
                 <c:pt idx="90" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9563295702195735E-2</c:v>
+                  <c:v>2.9563315055480266E-2</c:v>
                 </c:pt>
                 <c:pt idx="91" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.955845644595112E-2</c:v>
+                  <c:v>2.9558476193931038E-2</c:v>
                 </c:pt>
                 <c:pt idx="92" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9554001129239449E-2</c:v>
+                  <c:v>2.9553638122056247E-2</c:v>
                 </c:pt>
                 <c:pt idx="93" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9549171718618594E-2</c:v>
+                  <c:v>2.9549163510859122E-2</c:v>
                 </c:pt>
                 <c:pt idx="94" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9544343095443404E-2</c:v>
+                  <c:v>2.9544334757483082E-2</c:v>
                 </c:pt>
                 <c:pt idx="95" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9539515259430216E-2</c:v>
+                  <c:v>2.9539506791512182E-2</c:v>
                 </c:pt>
                 <c:pt idx="96" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.953468821057903E-2</c:v>
+                  <c:v>2.9534679612581716E-2</c:v>
                 </c:pt>
                 <c:pt idx="97" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9529861948606184E-2</c:v>
+                  <c:v>2.9529853220610636E-2</c:v>
                 </c:pt>
                 <c:pt idx="98" formatCode="0.0000;[Red]0.0000">
-                  <c:v>2.9525036473390109E-2</c:v>
+                  <c:v>2.952502761531528E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3667,7 +3675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3709,7 +3717,7 @@
       </c>
       <c r="B3" s="67">
         <f ca="1">TODAY()</f>
-        <v>43215</v>
+        <v>43640</v>
       </c>
       <c r="C3" s="30"/>
     </row>
@@ -3719,7 +3727,7 @@
       </c>
       <c r="B4" s="67">
         <f ca="1">B3</f>
-        <v>43215</v>
+        <v>43640</v>
       </c>
       <c r="C4" s="30"/>
     </row>
@@ -4120,7 +4128,7 @@
       </c>
       <c r="B2" s="9" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateAsset(Curves!A15, C39,Curves!B15, Curves!C15)</f>
-        <v>AUD-CPIndex-1D-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-1D-0.03-24/06/2019</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
@@ -4143,7 +4151,7 @@
       </c>
       <c r="B3" s="16" t="str">
         <f t="array" aca="1" ref="B3:B34" ca="1">_xll.HLV5r3.Financial.Cache.CreateAssets(Curves!A15:A35, C39, Curves!B15:B35, Curves!C15:C35)</f>
-        <v>AUD-CPIndex-1D-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-1D-0.03-24/06/2019</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>44</v>
@@ -4151,7 +4159,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="17" t="str">
         <f t="array" aca="1" ref="E3:N34" ca="1">_xll.HLV5r3.Financial.Cache.EvaluateMetricsForAssetSet(C2:C3, C37, B3:B23, C39)</f>
-        <v>AUD-CPIndex-1D-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-1D-0.03-24/06/2019</v>
       </c>
       <c r="F3" s="18" t="str">
         <f ca="1"/>
@@ -4194,13 +4202,13 @@
       <c r="A4" s="20"/>
       <c r="B4" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-1M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-1M-0.03-24/06/2019</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="21"/>
       <c r="E4" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-1M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-1M-0.03-24/06/2019</v>
       </c>
       <c r="F4" s="12" t="str">
         <f ca="1"/>
@@ -4243,13 +4251,13 @@
       <c r="A5" s="20"/>
       <c r="B5" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-2M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-2M-0.03-24/06/2019</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
       <c r="E5" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-2M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-2M-0.03-24/06/2019</v>
       </c>
       <c r="F5" s="12" t="str">
         <f ca="1"/>
@@ -4257,7 +4265,7 @@
       </c>
       <c r="G5" s="12">
         <f ca="1"/>
-        <v>3.0000000000003052E-2</v>
+        <v>2.9999999999998268E-2</v>
       </c>
       <c r="H5" s="12" t="str">
         <f ca="1"/>
@@ -4292,13 +4300,13 @@
       <c r="A6" s="20"/>
       <c r="B6" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-3M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-3M-0.03-24/06/2019</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
       <c r="E6" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-3M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-3M-0.03-24/06/2019</v>
       </c>
       <c r="F6" s="12" t="str">
         <f ca="1"/>
@@ -4306,7 +4314,7 @@
       </c>
       <c r="G6" s="12">
         <f ca="1"/>
-        <v>2.9999999999998566E-2</v>
+        <v>3.0000000000001192E-2</v>
       </c>
       <c r="H6" s="12" t="str">
         <f ca="1"/>
@@ -4341,13 +4349,13 @@
       <c r="A7" s="20"/>
       <c r="B7" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-4M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-4M-0.03-24/06/2019</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
       <c r="E7" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-4M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-4M-0.03-24/06/2019</v>
       </c>
       <c r="F7" s="12" t="str">
         <f ca="1"/>
@@ -4355,7 +4363,7 @@
       </c>
       <c r="G7" s="12">
         <f ca="1"/>
-        <v>2.9999999999998885E-2</v>
+        <v>2.9999999999999166E-2</v>
       </c>
       <c r="H7" s="12" t="str">
         <f ca="1"/>
@@ -4390,13 +4398,13 @@
       <c r="A8" s="20"/>
       <c r="B8" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-5M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-5M-0.03-24/06/2019</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
       <c r="E8" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-5M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-5M-0.03-24/06/2019</v>
       </c>
       <c r="F8" s="12" t="str">
         <f ca="1"/>
@@ -4404,7 +4412,7 @@
       </c>
       <c r="G8" s="12">
         <f ca="1"/>
-        <v>2.9999999999999152E-2</v>
+        <v>3.0000000000000693E-2</v>
       </c>
       <c r="H8" s="12" t="str">
         <f ca="1"/>
@@ -4439,13 +4447,13 @@
       <c r="A9" s="20"/>
       <c r="B9" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-6M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-6M-0.03-24/06/2019</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
       <c r="E9" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-CPIndex-6M-0.03-25/04/2018</v>
+        <v>AUD-CPIndex-6M-0.03-24/06/2019</v>
       </c>
       <c r="F9" s="12" t="str">
         <f ca="1"/>
@@ -4488,13 +4496,13 @@
       <c r="A10" s="20"/>
       <c r="B10" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-1Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-1Y-0.03-24/06/2019</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
       <c r="E10" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-1Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-1Y-0.03-24/06/2019</v>
       </c>
       <c r="F10" s="12" t="str">
         <f ca="1"/>
@@ -4537,13 +4545,13 @@
       <c r="A11" s="20"/>
       <c r="B11" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-2Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-2Y-0.03-24/06/2019</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
       <c r="E11" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-2Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-2Y-0.03-24/06/2019</v>
       </c>
       <c r="F11" s="12" t="str">
         <f ca="1"/>
@@ -4551,7 +4559,7 @@
       </c>
       <c r="G11" s="12">
         <f ca="1"/>
-        <v>3.0000000000000433E-2</v>
+        <v>2.9999999999999874E-2</v>
       </c>
       <c r="H11" s="12" t="str">
         <f ca="1"/>
@@ -4586,13 +4594,13 @@
       <c r="A12" s="20"/>
       <c r="B12" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-3Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-3Y-0.03-24/06/2019</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
       <c r="E12" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-3Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-3Y-0.03-24/06/2019</v>
       </c>
       <c r="F12" s="12" t="str">
         <f ca="1"/>
@@ -4635,13 +4643,13 @@
       <c r="A13" s="20"/>
       <c r="B13" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-4Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-4Y-0.03-24/06/2019</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-4Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-4Y-0.03-24/06/2019</v>
       </c>
       <c r="F13" s="12" t="str">
         <f ca="1"/>
@@ -4649,7 +4657,7 @@
       </c>
       <c r="G13" s="12">
         <f ca="1"/>
-        <v>2.9999999999999645E-2</v>
+        <v>3.000000000000027E-2</v>
       </c>
       <c r="H13" s="12" t="str">
         <f ca="1"/>
@@ -4684,13 +4692,13 @@
       <c r="A14" s="20"/>
       <c r="B14" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-5Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-5Y-0.03-24/06/2019</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
       <c r="E14" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-5Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-5Y-0.03-24/06/2019</v>
       </c>
       <c r="F14" s="12" t="str">
         <f ca="1"/>
@@ -4698,7 +4706,7 @@
       </c>
       <c r="G14" s="12">
         <f ca="1"/>
-        <v>3.0000000000000197E-2</v>
+        <v>2.9999999999999933E-2</v>
       </c>
       <c r="H14" s="12" t="str">
         <f ca="1"/>
@@ -4733,13 +4741,13 @@
       <c r="A15" s="20"/>
       <c r="B15" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-7Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-7Y-0.03-24/06/2019</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-7Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-7Y-0.03-24/06/2019</v>
       </c>
       <c r="F15" s="12" t="str">
         <f ca="1"/>
@@ -4747,7 +4755,7 @@
       </c>
       <c r="G15" s="12">
         <f ca="1"/>
-        <v>3.0000000000000252E-2</v>
+        <v>3.0000000000000457E-2</v>
       </c>
       <c r="H15" s="12" t="str">
         <f ca="1"/>
@@ -4782,13 +4790,13 @@
       <c r="A16" s="20"/>
       <c r="B16" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-8Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-8Y-0.03-24/06/2019</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
       <c r="E16" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-8Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-8Y-0.03-24/06/2019</v>
       </c>
       <c r="F16" s="12" t="str">
         <f ca="1"/>
@@ -4796,7 +4804,7 @@
       </c>
       <c r="G16" s="12">
         <f ca="1"/>
-        <v>3.0000000000000179E-2</v>
+        <v>3.0000000000000374E-2</v>
       </c>
       <c r="H16" s="12" t="str">
         <f ca="1"/>
@@ -4831,13 +4839,13 @@
       <c r="A17" s="20"/>
       <c r="B17" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-9Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-9Y-0.03-24/06/2019</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
       <c r="E17" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-9Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-9Y-0.03-24/06/2019</v>
       </c>
       <c r="F17" s="12" t="str">
         <f ca="1"/>
@@ -4845,7 +4853,7 @@
       </c>
       <c r="G17" s="12">
         <f ca="1"/>
-        <v>2.9999999999999669E-2</v>
+        <v>3.0000000000000207E-2</v>
       </c>
       <c r="H17" s="12" t="str">
         <f ca="1"/>
@@ -4880,13 +4888,13 @@
       <c r="A18" s="20"/>
       <c r="B18" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-10Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-10Y-0.03-24/06/2019</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
       <c r="E18" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-10Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-10Y-0.03-24/06/2019</v>
       </c>
       <c r="F18" s="12" t="str">
         <f ca="1"/>
@@ -4929,13 +4937,13 @@
       <c r="A19" s="20"/>
       <c r="B19" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-12Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-12Y-0.03-24/06/2019</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
       <c r="E19" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-12Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-12Y-0.03-24/06/2019</v>
       </c>
       <c r="F19" s="12" t="str">
         <f ca="1"/>
@@ -4978,13 +4986,13 @@
       <c r="A20" s="20"/>
       <c r="B20" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-15Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-15Y-0.03-24/06/2019</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
       <c r="E20" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-15Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-15Y-0.03-24/06/2019</v>
       </c>
       <c r="F20" s="12" t="str">
         <f ca="1"/>
@@ -4992,7 +5000,7 @@
       </c>
       <c r="G20" s="12">
         <f ca="1"/>
-        <v>2.999999999999951E-2</v>
+        <v>3.0000000000000211E-2</v>
       </c>
       <c r="H20" s="12" t="str">
         <f ca="1"/>
@@ -5027,13 +5035,13 @@
       <c r="A21" s="20"/>
       <c r="B21" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-20Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-20Y-0.03-24/06/2019</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
       <c r="E21" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-20Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-20Y-0.03-24/06/2019</v>
       </c>
       <c r="F21" s="12" t="str">
         <f ca="1"/>
@@ -5041,7 +5049,7 @@
       </c>
       <c r="G21" s="12">
         <f ca="1"/>
-        <v>3.0000000000000641E-2</v>
+        <v>2.9999999999999617E-2</v>
       </c>
       <c r="H21" s="12" t="str">
         <f ca="1"/>
@@ -5076,13 +5084,13 @@
       <c r="A22" s="20"/>
       <c r="B22" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-25Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-25Y-0.03-24/06/2019</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
       <c r="E22" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-25Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-25Y-0.03-24/06/2019</v>
       </c>
       <c r="F22" s="12" t="str">
         <f ca="1"/>
@@ -5090,7 +5098,7 @@
       </c>
       <c r="G22" s="12">
         <f ca="1"/>
-        <v>3.0000000000000544E-2</v>
+        <v>2.9999999999999933E-2</v>
       </c>
       <c r="H22" s="12" t="str">
         <f ca="1"/>
@@ -5125,13 +5133,13 @@
       <c r="A23" s="20"/>
       <c r="B23" s="16" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-30Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-30Y-0.03-24/06/2019</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
       <c r="E23" s="22" t="str">
         <f ca="1"/>
-        <v>AUD-ZCCPISwap-30Y-0.03-25/04/2018</v>
+        <v>AUD-ZCCPISwap-30Y-0.03-24/06/2019</v>
       </c>
       <c r="F23" s="12" t="str">
         <f ca="1"/>
@@ -5139,7 +5147,7 @@
       </c>
       <c r="G23" s="12">
         <f ca="1"/>
-        <v>2.9999999999999648E-2</v>
+        <v>3.0000000000000249E-2</v>
       </c>
       <c r="H23" s="12" t="str">
         <f ca="1"/>
@@ -5733,7 +5741,7 @@
       </c>
       <c r="C39" s="75">
         <f ca="1">Curves!B3</f>
-        <v>43215</v>
+        <v>43640</v>
       </c>
     </row>
   </sheetData>
@@ -5748,7 +5756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -5778,7 +5786,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="45">
         <f ca="1">Curves!B3</f>
-        <v>43215</v>
+        <v>43640</v>
       </c>
       <c r="B2" s="46">
         <f ca="1">B3</f>
@@ -5793,7 +5801,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="49">
         <f t="shared" ref="A3:A67" ca="1" si="0">A2+1</f>
-        <v>43216</v>
+        <v>43641</v>
       </c>
       <c r="B3" s="50">
         <f ca="1">(D2-D3)/(A3-A2)*365</f>
@@ -5808,7 +5816,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43217</v>
+        <v>43642</v>
       </c>
       <c r="B4" s="51">
         <f t="shared" ref="B4:B67" ca="1" si="1">(D3-D4)/(A4-A3)*365</f>
@@ -5823,7 +5831,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43218</v>
+        <v>43643</v>
       </c>
       <c r="B5" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5838,7 +5846,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43219</v>
+        <v>43644</v>
       </c>
       <c r="B6" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5853,7 +5861,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43220</v>
+        <v>43645</v>
       </c>
       <c r="B7" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5868,7 +5876,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43221</v>
+        <v>43646</v>
       </c>
       <c r="B8" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5883,7 +5891,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43222</v>
+        <v>43647</v>
       </c>
       <c r="B9" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5898,7 +5906,7 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43223</v>
+        <v>43648</v>
       </c>
       <c r="B10" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5913,7 +5921,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43224</v>
+        <v>43649</v>
       </c>
       <c r="B11" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5928,7 +5936,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43225</v>
+        <v>43650</v>
       </c>
       <c r="B12" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5943,7 +5951,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43226</v>
+        <v>43651</v>
       </c>
       <c r="B13" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5958,7 +5966,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43227</v>
+        <v>43652</v>
       </c>
       <c r="B14" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5973,7 +5981,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43228</v>
+        <v>43653</v>
       </c>
       <c r="B15" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -5988,7 +5996,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43229</v>
+        <v>43654</v>
       </c>
       <c r="B16" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6003,7 +6011,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43230</v>
+        <v>43655</v>
       </c>
       <c r="B17" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6018,7 +6026,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43231</v>
+        <v>43656</v>
       </c>
       <c r="B18" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6033,7 +6041,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43232</v>
+        <v>43657</v>
       </c>
       <c r="B19" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6048,7 +6056,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43233</v>
+        <v>43658</v>
       </c>
       <c r="B20" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6063,7 +6071,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43234</v>
+        <v>43659</v>
       </c>
       <c r="B21" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6078,7 +6086,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43235</v>
+        <v>43660</v>
       </c>
       <c r="B22" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6093,7 +6101,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43236</v>
+        <v>43661</v>
       </c>
       <c r="B23" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6108,7 +6116,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43237</v>
+        <v>43662</v>
       </c>
       <c r="B24" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6123,7 +6131,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43238</v>
+        <v>43663</v>
       </c>
       <c r="B25" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6138,7 +6146,7 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43239</v>
+        <v>43664</v>
       </c>
       <c r="B26" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6153,7 +6161,7 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43240</v>
+        <v>43665</v>
       </c>
       <c r="B27" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6168,7 +6176,7 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43241</v>
+        <v>43666</v>
       </c>
       <c r="B28" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6183,7 +6191,7 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43242</v>
+        <v>43667</v>
       </c>
       <c r="B29" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6198,7 +6206,7 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43243</v>
+        <v>43668</v>
       </c>
       <c r="B30" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6213,7 +6221,7 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43244</v>
+        <v>43669</v>
       </c>
       <c r="B31" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6228,7 +6236,7 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43245</v>
+        <v>43670</v>
       </c>
       <c r="B32" s="51">
         <f t="shared" ca="1" si="1"/>
@@ -6243,1021 +6251,1021 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43246</v>
+        <v>43671</v>
       </c>
       <c r="B33" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9850215165305727E-2</v>
+        <v>2.9850219315280535E-2</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A33)</f>
-        <v>0.99745853014912422</v>
+        <v>0.99745853013775443</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43247</v>
+        <v>43672</v>
       </c>
       <c r="B34" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9845320876650816E-2</v>
+        <v>2.9845325293673119E-2</v>
       </c>
       <c r="C34" s="47"/>
       <c r="D34" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A34)</f>
-        <v>0.99737676214672244</v>
+        <v>0.99737676212325121</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43248</v>
+        <v>43673</v>
       </c>
       <c r="B35" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.984042738938153E-2</v>
+        <v>2.9840432073289236E-2</v>
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A35)</f>
-        <v>0.99729500755113509</v>
+        <v>0.99729500751483124</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43249</v>
+        <v>43674</v>
       </c>
       <c r="B36" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.983553470313316E-2</v>
+        <v>2.9835539654047838E-2</v>
       </c>
       <c r="C36" s="47"/>
       <c r="D36" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A36)</f>
-        <v>0.99721326636016761</v>
+        <v>0.99721326631029961</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43250</v>
+        <v>43675</v>
       </c>
       <c r="B37" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9830642817986752E-2</v>
+        <v>2.9830648035665264E-2</v>
       </c>
       <c r="C37" s="47"/>
       <c r="D37" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A37)</f>
-        <v>0.99713153857162518</v>
+        <v>0.99713153850746217</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43251</v>
+        <v>43676</v>
       </c>
       <c r="B38" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9825751733618122E-2</v>
+        <v>2.982575721810099E-2</v>
       </c>
       <c r="C38" s="47"/>
       <c r="D38" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A38)</f>
-        <v>0.99704982418331389</v>
+        <v>0.9970498241041249</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43252</v>
+        <v>43677</v>
       </c>
       <c r="B39" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9820861449865177E-2</v>
+        <v>2.9820867201111878E-2</v>
       </c>
       <c r="C39" s="47"/>
       <c r="D39" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A39)</f>
-        <v>0.99696812319304029</v>
+        <v>0.99696812309809446</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43253</v>
+        <v>43678</v>
       </c>
       <c r="B40" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9815971966606347E-2</v>
+        <v>2.9815977984495312E-2</v>
       </c>
       <c r="C40" s="47"/>
       <c r="D40" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A40)</f>
-        <v>0.99688643559861123</v>
+        <v>0.99688643548717804</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43254</v>
+        <v>43679</v>
       </c>
       <c r="B41" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9811083283760587E-2</v>
+        <v>2.9811089568210769E-2</v>
       </c>
       <c r="C41" s="47"/>
       <c r="D41" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A41)</f>
-        <v>0.99680476139783381</v>
+        <v>0.99680476126918294</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43255</v>
+        <v>43680</v>
       </c>
       <c r="B42" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.980619540100371E-2</v>
+        <v>2.9806201951974587E-2</v>
       </c>
       <c r="C42" s="47"/>
       <c r="D42" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A42)</f>
-        <v>0.99672310058851599</v>
+        <v>0.99672310044191725</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43256</v>
+        <v>43681</v>
       </c>
       <c r="B43" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9801308318295194E-2</v>
+        <v>2.9801315135705719E-2</v>
       </c>
       <c r="C43" s="47"/>
       <c r="D43" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A43)</f>
-        <v>0.99664145316846586</v>
+        <v>0.99664145300318929</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43257</v>
+        <v>43682</v>
       </c>
       <c r="B44" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9796422035351378E-2</v>
+        <v>2.9796429119161028E-2</v>
       </c>
       <c r="C44" s="47"/>
       <c r="D44" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A44)</f>
-        <v>0.9965598191354923</v>
+        <v>0.99655981895080803</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43258</v>
+        <v>43683</v>
       </c>
       <c r="B45" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9791536552131737E-2</v>
+        <v>2.9791543902218942E-2</v>
       </c>
       <c r="C45" s="47"/>
       <c r="D45" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A45)</f>
-        <v>0.99647819848740427</v>
+        <v>0.99647819828258277</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43259</v>
+        <v>43684</v>
       </c>
       <c r="B46" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9786651868433656E-2</v>
+        <v>2.9786659484798417E-2</v>
       </c>
       <c r="C46" s="47"/>
       <c r="D46" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A46)</f>
-        <v>0.9963965912220113</v>
+        <v>0.99639659099632305</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43260</v>
+        <v>43685</v>
       </c>
       <c r="B47" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9781767984054519E-2</v>
+        <v>2.9781775866615789E-2</v>
       </c>
       <c r="C47" s="47"/>
       <c r="D47" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A47)</f>
-        <v>0.99631499733712348</v>
+        <v>0.99631499708983917</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43261</v>
+        <v>43686</v>
       </c>
       <c r="B48" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9776884898832234E-2</v>
+        <v>2.9776893047549491E-2</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A48)</f>
-        <v>0.99623341683055133</v>
+        <v>0.99623341656094178</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43262</v>
+        <v>43687</v>
       </c>
       <c r="B49" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9772002612685755E-2</v>
+        <v>2.9772011027396905E-2</v>
       </c>
       <c r="C49" s="47"/>
       <c r="D49" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A49)</f>
-        <v>0.99615184970010562</v>
+        <v>0.99615184940744206</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43263</v>
+        <v>43688</v>
       </c>
       <c r="B50" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9767121125331419E-2</v>
+        <v>2.9767129806117509E-2</v>
       </c>
       <c r="C50" s="47"/>
       <c r="D50" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A50)</f>
-        <v>0.99607029594359786</v>
+        <v>0.99607029562715133</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43264</v>
+        <v>43689</v>
       </c>
       <c r="B51" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9762240436688181E-2</v>
+        <v>2.9762249383387118E-2</v>
       </c>
       <c r="C51" s="47"/>
       <c r="D51" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A51)</f>
-        <v>0.99598875555883981</v>
+        <v>0.99598875521788177</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43265</v>
+        <v>43690</v>
       </c>
       <c r="B52" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.975736054663447E-2</v>
+        <v>2.9757369759124686E-2</v>
       </c>
       <c r="C52" s="47"/>
       <c r="D52" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A52)</f>
-        <v>0.99590722854364355</v>
+        <v>0.99590722817744581</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43266</v>
+        <v>43691</v>
       </c>
       <c r="B53" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9752481454846103E-2</v>
+        <v>2.9752490933168119E-2</v>
       </c>
       <c r="C53" s="47"/>
       <c r="D53" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A53)</f>
-        <v>0.99582571489582206</v>
+        <v>0.99582571450365631</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43267</v>
+        <v>43692</v>
       </c>
       <c r="B54" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9747603161323077E-2</v>
+        <v>2.9747612905395848E-2</v>
       </c>
       <c r="C54" s="47"/>
       <c r="D54" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A54)</f>
-        <v>0.99574421461318829</v>
+        <v>0.99574421419432646</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43268</v>
+        <v>43693</v>
       </c>
       <c r="B55" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.974272566574121E-2</v>
+        <v>2.9742735675564735E-2</v>
       </c>
       <c r="C55" s="47"/>
       <c r="D55" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A55)</f>
-        <v>0.99566272769355613</v>
+        <v>0.99566272724727012</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43269</v>
+        <v>43694</v>
       </c>
       <c r="B56" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9737848968181546E-2</v>
+        <v>2.9737859243512688E-2</v>
       </c>
       <c r="C56" s="47"/>
       <c r="D56" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A56)</f>
-        <v>0.99558125413473919</v>
+        <v>0.99558125366030159</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43270</v>
+        <v>43695</v>
       </c>
       <c r="B57" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9732973068238855E-2</v>
+        <v>2.9732983609158659E-2</v>
       </c>
       <c r="C57" s="47"/>
       <c r="D57" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A57)</f>
-        <v>0.99549979393455224</v>
+        <v>0.9954997934312354</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43271</v>
+        <v>43696</v>
       </c>
       <c r="B58" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9728097965872613E-2</v>
+        <v>2.9728108772218986E-2</v>
       </c>
       <c r="C58" s="47"/>
       <c r="D58" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A58)</f>
-        <v>0.99541834709081012</v>
+        <v>0.99541834655788686</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43272</v>
+        <v>43697</v>
       </c>
       <c r="B59" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9723223660880205E-2</v>
+        <v>2.9723234732653148E-2</v>
       </c>
       <c r="C59" s="47"/>
       <c r="D59" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A59)</f>
-        <v>0.99533691360132825</v>
+        <v>0.99533691303807137</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43273</v>
+        <v>43698</v>
       </c>
       <c r="B60" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9718350153099538E-2</v>
+        <v>2.9718361490218004E-2</v>
       </c>
       <c r="C60" s="47"/>
       <c r="D60" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A60)</f>
-        <v>0.9952554934639225</v>
+        <v>0.99525549286960502</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43274</v>
+        <v>43699</v>
       </c>
       <c r="B61" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9713477442368519E-2</v>
+        <v>2.9713489044751462E-2</v>
       </c>
       <c r="C61" s="47"/>
       <c r="D61" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A61)</f>
-        <v>0.99517408667640916</v>
+        <v>0.99517408605030433</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43275</v>
+        <v>43700</v>
       </c>
       <c r="B62" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9708605528525056E-2</v>
+        <v>2.9708617396172476E-2</v>
       </c>
       <c r="C62" s="47"/>
       <c r="D62" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A62)</f>
-        <v>0.99509269323660499</v>
+        <v>0.99509269257798605</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43276</v>
+        <v>43701</v>
       </c>
       <c r="B63" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.970373441144758E-2</v>
+        <v>2.9703746544197385E-2</v>
       </c>
       <c r="C63" s="47"/>
       <c r="D63" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A63)</f>
-        <v>0.99501131314232705</v>
+        <v>0.9950113124504677</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43277</v>
+        <v>43702</v>
       </c>
       <c r="B64" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9699116165411987E-2</v>
+        <v>2.9698876488785664E-2</v>
       </c>
       <c r="C64" s="47"/>
       <c r="D64" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A64)</f>
-        <v>0.99492994570077797</v>
+        <v>0.99492994566556692</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43278</v>
+        <v>43703</v>
       </c>
       <c r="B65" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9694254730974201E-2</v>
+        <v>2.9694007229694175E-2</v>
       </c>
       <c r="C65" s="47"/>
       <c r="D65" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A65)</f>
-        <v>0.99484859157822736</v>
+        <v>0.994848592221102</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43279</v>
+        <v>43704</v>
       </c>
       <c r="B66" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9689394090789967E-2</v>
+        <v>2.9689403146496152E-2</v>
       </c>
       <c r="C66" s="47"/>
       <c r="D66" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A66)</f>
-        <v>0.99476725077249917</v>
+        <v>0.99476725139056366</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="49">
         <f t="shared" ca="1" si="0"/>
-        <v>43280</v>
+        <v>43705</v>
       </c>
       <c r="B67" s="51">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9684534244697192E-2</v>
+        <v>2.9684543697732768E-2</v>
       </c>
       <c r="C67" s="47"/>
       <c r="D67" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A67)</f>
-        <v>0.99468592328141781</v>
+        <v>0.99468592387358357</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="49">
         <f t="shared" ref="A68:A100" ca="1" si="2">A67+1</f>
-        <v>43281</v>
+        <v>43706</v>
       </c>
       <c r="B68" s="51">
         <f t="shared" ref="B68:B100" ca="1" si="3">(D67-D68)/(A68-A67)*365</f>
-        <v>2.9679675192655353E-2</v>
+        <v>2.9679685042777182E-2</v>
       </c>
       <c r="C68" s="47"/>
       <c r="D68" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A68)</f>
-        <v>0.99460460910280779</v>
+        <v>0.99460460966798692</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43282</v>
+        <v>43707</v>
       </c>
       <c r="B69" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9674816934299741E-2</v>
+        <v>2.967482718158887E-2</v>
       </c>
       <c r="C69" s="47"/>
       <c r="D69" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A69)</f>
-        <v>0.99452330823449464</v>
+        <v>0.994523308771599</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43283</v>
+        <v>43708</v>
       </c>
       <c r="B70" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9669959469589835E-2</v>
+        <v>2.96699701137626E-2</v>
       </c>
       <c r="C70" s="47"/>
       <c r="D70" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A70)</f>
-        <v>0.99444202067430398</v>
+        <v>0.99444202118224623</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43284</v>
+        <v>43709</v>
       </c>
       <c r="B71" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9665102798282494E-2</v>
+        <v>2.9665113839419943E-2</v>
       </c>
       <c r="C71" s="47"/>
       <c r="D71" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A71)</f>
-        <v>0.99436074642006211</v>
+        <v>0.99436074689775467</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43285</v>
+        <v>43710</v>
       </c>
       <c r="B72" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9660246920337197E-2</v>
+        <v>2.9660258358155667E-2</v>
       </c>
       <c r="C72" s="47"/>
       <c r="D72" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A72)</f>
-        <v>0.99427948546959544</v>
+        <v>0.9942794859159515</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43286</v>
+        <v>43711</v>
       </c>
       <c r="B73" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9655391835470279E-2</v>
+        <v>2.9655403670050817E-2</v>
       </c>
       <c r="C73" s="47"/>
       <c r="D73" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A73)</f>
-        <v>0.99419823782073113</v>
+        <v>0.99419823823466369</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43287</v>
+        <v>43712</v>
       </c>
       <c r="B74" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9650537543560174E-2</v>
+        <v>2.9650549774700163E-2</v>
       </c>
       <c r="C74" s="47"/>
       <c r="D74" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A74)</f>
-        <v>0.99411700347129672</v>
+        <v>0.99411700385171931</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43288</v>
+        <v>43713</v>
       </c>
       <c r="B75" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9645684044444787E-2</v>
+        <v>2.9645696672144228E-2</v>
       </c>
       <c r="C75" s="47"/>
       <c r="D75" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A75)</f>
-        <v>0.99403578241912016</v>
+        <v>0.99403578276494631</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43289</v>
+        <v>43714</v>
       </c>
       <c r="B76" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9640831338043072E-2</v>
+        <v>2.964084436209935E-2</v>
       </c>
       <c r="C76" s="47"/>
       <c r="D76" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A76)</f>
-        <v>0.99395457466202963</v>
+        <v>0.99395457497217343</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43290</v>
+        <v>43715</v>
       </c>
       <c r="B77" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9635979424111891E-2</v>
+        <v>2.9635992844484482E-2</v>
       </c>
       <c r="C77" s="47"/>
       <c r="D77" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A77)</f>
-        <v>0.99387338019785398</v>
+        <v>0.99387338047122964</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43291</v>
+        <v>43716</v>
       </c>
       <c r="B78" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9631128302448628E-2</v>
+        <v>2.9631142119015963E-2</v>
       </c>
       <c r="C78" s="47"/>
       <c r="D78" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A78)</f>
-        <v>0.99379219902442262</v>
+        <v>0.99379219925994466</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43292</v>
+        <v>43717</v>
       </c>
       <c r="B79" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9626277972972237E-2</v>
+        <v>2.9626292185612746E-2</v>
       </c>
       <c r="C79" s="47"/>
       <c r="D79" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A79)</f>
-        <v>0.99371103113956516</v>
+        <v>0.99371103133614846</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43293</v>
+        <v>43718</v>
       </c>
       <c r="B80" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9621428435480102E-2</v>
+        <v>2.9621443044112739E-2</v>
       </c>
       <c r="C80" s="47"/>
       <c r="D80" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A80)</f>
-        <v>0.99362987654111179</v>
+        <v>0.99362987669767144</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43294</v>
+        <v>43719</v>
       </c>
       <c r="B81" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.961657968981013E-2</v>
+        <v>2.9616594694394371E-2</v>
       </c>
       <c r="C81" s="47"/>
       <c r="D81" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A81)</f>
-        <v>0.99354873522689313</v>
+        <v>0.99354873534234434</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43295</v>
+        <v>43720</v>
       </c>
       <c r="B82" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9611731735759705E-2</v>
+        <v>2.9611747136214506E-2</v>
       </c>
       <c r="C82" s="47"/>
       <c r="D82" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A82)</f>
-        <v>0.99346760719474037</v>
+        <v>0.99346760726799854</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43296</v>
+        <v>43721</v>
       </c>
       <c r="B83" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9606884573328829E-2</v>
+        <v>2.9606900369451572E-2</v>
       </c>
       <c r="C83" s="47"/>
       <c r="D83" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A83)</f>
-        <v>0.99338649244248467</v>
+        <v>0.9933864924724658</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43297</v>
+        <v>43722</v>
       </c>
       <c r="B84" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9602038202233838E-2</v>
+        <v>2.9602054394024524E-2</v>
       </c>
       <c r="C84" s="47"/>
       <c r="D84" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A84)</f>
-        <v>0.993305390967958</v>
+        <v>0.99330539095357806</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43298</v>
+        <v>43723</v>
       </c>
       <c r="B85" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9597192622231594E-2</v>
+        <v>2.959720920952813E-2</v>
       </c>
       <c r="C85" s="47"/>
       <c r="D85" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A85)</f>
-        <v>0.99322430276899298</v>
+        <v>0.99322430270916839</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43299</v>
+        <v>43724</v>
       </c>
       <c r="B86" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.959234783336262E-2</v>
+        <v>2.9592364816002914E-2</v>
       </c>
       <c r="C86" s="47"/>
       <c r="D86" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A86)</f>
-        <v>0.99314322784342213</v>
+        <v>0.99314322773706976</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43300</v>
+        <v>43725</v>
       </c>
       <c r="B87" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9587503835262208E-2</v>
+        <v>2.9587521213327306E-2</v>
       </c>
       <c r="C87" s="47"/>
       <c r="D87" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A87)</f>
-        <v>0.99306216618907894</v>
+        <v>0.99306216603511543</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43301</v>
+        <v>43726</v>
       </c>
       <c r="B88" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9582660627930357E-2</v>
+        <v>2.958267840117712E-2</v>
       </c>
       <c r="C88" s="47"/>
       <c r="D88" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A88)</f>
-        <v>0.99298111780379694</v>
+        <v>0.99298111760113961</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43302</v>
+        <v>43727</v>
       </c>
       <c r="B89" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9577818211083406E-2</v>
+        <v>2.9577836379471312E-2</v>
       </c>
       <c r="C89" s="47"/>
       <c r="D89" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A89)</f>
-        <v>0.99290008268541041</v>
+        <v>0.99290008243297667</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43303</v>
+        <v>43728</v>
       </c>
       <c r="B90" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9572976584559263E-2</v>
+        <v>2.957299514808831E-2</v>
       </c>
       <c r="C90" s="47"/>
       <c r="D90" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A90)</f>
-        <v>0.99281906083175409</v>
+        <v>0.99281906052846136</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43304</v>
+        <v>43729</v>
       </c>
       <c r="B91" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.956813574839845E-2</v>
+        <v>2.9568154706906546E-2</v>
       </c>
       <c r="C91" s="47"/>
       <c r="D91" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A91)</f>
-        <v>0.99273805224066258</v>
+        <v>0.99273805188542874</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43305</v>
+        <v>43730</v>
       </c>
       <c r="B92" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9563295702195735E-2</v>
+        <v>2.9563315055480266E-2</v>
       </c>
       <c r="C92" s="47"/>
       <c r="D92" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A92)</f>
-        <v>0.99265705690997164</v>
+        <v>0.9926570565017151</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43306</v>
+        <v>43731</v>
       </c>
       <c r="B93" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.955845644595112E-2</v>
+        <v>2.9558476193931038E-2</v>
       </c>
       <c r="C93" s="47"/>
       <c r="D93" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A93)</f>
-        <v>0.99257607483751698</v>
+        <v>0.99257607437515638</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43307</v>
+        <v>43732</v>
       </c>
       <c r="B94" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9554001129239449E-2</v>
+        <v>2.9553638122056247E-2</v>
       </c>
       <c r="C94" s="47"/>
       <c r="D94" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A94)</f>
-        <v>0.99249510497140947</v>
+        <v>0.9924951055035891</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43308</v>
+        <v>43733</v>
       </c>
       <c r="B95" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9549171718618594E-2</v>
+        <v>2.9549163510859122E-2</v>
       </c>
       <c r="C95" s="47"/>
       <c r="D95" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A95)</f>
-        <v>0.99241414833656394</v>
+        <v>0.99241414889123059</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43309</v>
+        <v>43734</v>
       </c>
       <c r="B96" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9544343095443404E-2</v>
+        <v>2.9544334757483082E-2</v>
       </c>
       <c r="C96" s="47"/>
       <c r="D96" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A96)</f>
-        <v>0.992333204930823</v>
+        <v>0.99233320550833337</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43310</v>
+        <v>43735</v>
       </c>
       <c r="B97" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9539515259430216E-2</v>
+        <v>2.9539506791512182E-2</v>
       </c>
       <c r="C97" s="47"/>
       <c r="D97" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A97)</f>
-        <v>0.99225227475203004</v>
+        <v>0.99225227535274019</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43311</v>
+        <v>43736</v>
       </c>
       <c r="B98" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.953468821057903E-2</v>
+        <v>2.9534679612581716E-2</v>
       </c>
       <c r="C98" s="47"/>
       <c r="D98" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A98)</f>
-        <v>0.99217135779802845</v>
+        <v>0.99217135842229476</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="49">
         <f t="shared" ca="1" si="2"/>
-        <v>43312</v>
+        <v>43737</v>
       </c>
       <c r="B99" s="51">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9529861948606184E-2</v>
+        <v>2.9529853220610636E-2</v>
       </c>
       <c r="C99" s="47"/>
       <c r="D99" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A99)</f>
-        <v>0.99209045406666241</v>
+        <v>0.99209045471484103</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="52">
         <f t="shared" ca="1" si="2"/>
-        <v>43313</v>
+        <v>43738</v>
       </c>
       <c r="B100" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9525036473390109E-2</v>
+        <v>2.952502761531528E-2</v>
       </c>
       <c r="C100" s="54"/>
       <c r="D100" s="48">
         <f ca="1">_xll.HLV5r3.Financial.Cache.GetValue(Curves!$B$1, 'Daily Forward Rates'!A100)</f>
-        <v>0.99200956355577641</v>
+        <v>0.99200956422822373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>